<commit_message>
Problem of extra column Study parameters:
Due to splitting study parameters in two columns, a small problem arose when selecting them. Also now the program has less folders it needs to go through
</commit_message>
<xml_diff>
--- a/Results/Book1.xlsx
+++ b/Results/Book1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,33 +461,272 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>AVG Offset Radial (mm)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>STD Offset Radial (mm)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>kVp</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Kernel</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Folder</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Path</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Manufacturer</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Channels</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>GNL 10 SLICE</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D2" t="n">
+        <v>128.4</v>
+      </c>
+      <c r="E2" t="n">
+        <v>119.748235895148</v>
+      </c>
+      <c r="F2" t="n">
+        <v>44.40787540013459</v>
+      </c>
+      <c r="G2" t="n">
+        <v>4.047788885572326</v>
+      </c>
+      <c r="H2" t="n">
+        <v>100</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Br54d</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>CT11_Lung</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>D:\Ani Nikoghosyan - CT11 vs CT14\Data\Studie_001\CT11_Lung</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>SIEMENS</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>SOMATOM Force</t>
+        </is>
+      </c>
+      <c r="N2" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>GNL 10 SLICE</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" t="n">
+        <v>130.9</v>
+      </c>
+      <c r="E3" t="n">
+        <v>122.9613353863726</v>
+      </c>
+      <c r="F3" t="n">
+        <v>44.48638906461505</v>
+      </c>
+      <c r="G3" t="n">
+        <v>4.071368516985725</v>
+      </c>
+      <c r="H3" t="n">
+        <v>100</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Br40d</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>CT11_Soft</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>D:\Ani Nikoghosyan - CT11 vs CT14\Data\Studie_001\CT11_Soft</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>SIEMENS</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>SOMATOM Force</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>GNL 10 SLICE</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D4" t="n">
+        <v>38.9</v>
+      </c>
+      <c r="E4" t="n">
+        <v>18.65180956368577</v>
+      </c>
+      <c r="F4" t="n">
+        <v>6.003067895637413</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3.722010148867418</v>
+      </c>
+      <c r="H4" t="n">
+        <v>120</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Bl56f</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>CT14_Lung</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>D:\Ani Nikoghosyan - CT11 vs CT14\Data\Studie_001\CT14_Lung</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Siemens Healthineers</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>NAEOTOM Alpha</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>GNL 10 SLICE</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>10</v>
+      </c>
+      <c r="D5" t="n">
+        <v>39.1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>18.96549498431296</v>
+      </c>
+      <c r="F5" t="n">
+        <v>6.498821079299242</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3.741648288920148</v>
+      </c>
+      <c r="H5" t="n">
+        <v>120</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Br40f</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>CT14_Soft</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>D:\Ani Nikoghosyan - CT11 vs CT14\Data\Studie_001\CT14_Soft</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Siemens Healthineers</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>NAEOTOM Alpha</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last extra updates. Don't really know what they were. But yeah here they are committed
</commit_message>
<xml_diff>
--- a/Results/Book1.xlsx
+++ b/Results/Book1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:CD2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,47 +461,387 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>AVG mA</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>STD mA</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>AVG CTDI (mGy)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>STD CTDI (mGy)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>AVG SSDE (mGy)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>STD SSDE (mGy)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>AVG WED (cm)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>STD WED (cm)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>AVG Truncation Correction</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>STD Truncation Correction</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>AVG Truncation Fraction</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>STD Truncation Fraction</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>AVG Body Area (cm²)</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>STD Body Area (cm²)</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>AVG Reconstruction Diameter (mm)</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>STD Reconstruction Diameter (mm)</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>AVG Collection Diameter (mm)</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>STD Collection Diameter (mm)</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>AVG Offset Horizontal (mm)</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>STD Offset Horizontal (mm)</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>AVG Offset Vertical (mm)</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>STD Offset Vertical (mm)</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
           <t>AVG Offset Radial (mm)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>STD Offset Radial (mm)</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>AVG GNL Soft Tissue - ST 3mm (HU)</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>STD GNL Soft Tissue - ST 3mm (HU)</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>AVG GNL Soft Tissue (HU)</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>STD GNL Soft Tissue (HU)</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Soft Tissue - Low (HU)</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Soft Tissue - High (HU)</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>AVG Soft Tissue Area (cm²)</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>STD Soft Tissue Area (cm²)</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>AVG Soft Tissue in body (%)</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>STD Soft Tissue in body (%)</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>AVG GNL Lung Tissue - ST 3mm (HU)</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>STD GNL Lung Tissue - ST 3mm (HU)</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>AVG GNL Lung Tissue (HU)</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>STD GNL Lung Tissue (HU)</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>Lung Tissue - Low (HU)</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Lung Tissue - High (HU)</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>AVG Lung Tissue Area (cm²)</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>STD Lung Tissue Area (cm²)</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>AVG Lung Tissue in body (%)</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>STD Lung Tissue in body (%)</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>Mask Kernel (mm)</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>Mask Kernel (px)</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>kVp</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>Kernel</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>FOV (mm)</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>Slice Thickness (mm)</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>Pixel Size (mm)</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>Pitch</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>Protocol</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>Procedure</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>Total Collimation (mm)</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>Single Collimation (mm)</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>Study Date</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>Exposure Time (ms)</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>Revolution Time (s)</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
         <is>
           <t>Folder</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>Matrix Size</t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
+          <t>Study Comments</t>
+        </is>
+      </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>Study Description</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
         <is>
           <t>Path</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>PACSID</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
         <is>
           <t>Manufacturer</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="BT1" s="1" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>Station</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
         <is>
           <t>Channels</t>
+        </is>
+      </c>
+      <c r="BW1" s="1" t="inlineStr">
+        <is>
+          <t>Software Version</t>
+        </is>
+      </c>
+      <c r="BX1" s="1" t="inlineStr">
+        <is>
+          <t>Filter Type</t>
+        </is>
+      </c>
+      <c r="BY1" s="1" t="inlineStr">
+        <is>
+          <t>Exposure Modulation Type</t>
+        </is>
+      </c>
+      <c r="BZ1" s="1" t="inlineStr">
+        <is>
+          <t>Acquisition Type</t>
+        </is>
+      </c>
+      <c r="CA1" s="1" t="inlineStr">
+        <is>
+          <t>Patient Sex</t>
+        </is>
+      </c>
+      <c r="CB1" s="1" t="inlineStr">
+        <is>
+          <t>Patient Age (y)</t>
+        </is>
+      </c>
+      <c r="CC1" s="1" t="inlineStr">
+        <is>
+          <t>Body Part Examined</t>
+        </is>
+      </c>
+      <c r="CD1" s="1" t="inlineStr">
+        <is>
+          <t>Patient ID</t>
         </is>
       </c>
     </row>
@@ -511,222 +851,230 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>GNL 10 SLICE</t>
+          <t>GNL X SLICE</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D2" t="n">
-        <v>128.4</v>
+        <v>40</v>
       </c>
       <c r="E2" t="n">
-        <v>119.748235895148</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>44.40787540013459</v>
+        <v>150</v>
       </c>
       <c r="G2" t="n">
-        <v>4.047788885572326</v>
-      </c>
-      <c r="H2" t="n">
-        <v>100</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Br54d</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>CT11_Lung</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>D:\Ani Nikoghosyan - CT11 vs CT14\Data\Studie_001\CT11_Lung</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="n">
+        <v>24.13026586602127</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1.74312419506365</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1.014673598249369</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.01314057548184452</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.1943118009848881</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.09757812955721759</v>
+      </c>
+      <c r="R2" t="n">
+        <v>595.8851165771484</v>
+      </c>
+      <c r="S2" t="n">
+        <v>62.2120997865178</v>
+      </c>
+      <c r="T2" t="n">
+        <v>300</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="n">
+        <v>49.05511458213778</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>12.34810646752503</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>60.08</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>15.12328006749858</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>170</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>164.7314071655273</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>51.74621522409029</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.2803269487782276</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.09120930950228189</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>48.71762932868766</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>7.472647177570734</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>59.66666666666666</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>9.152086306448588</v>
+      </c>
+      <c r="AR2" t="inlineStr">
+        <is>
+          <t>-inf</t>
+        </is>
+      </c>
+      <c r="AS2" t="n">
+        <v>-600</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>178.8395690917969</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>114.6557103856391</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>0.2873481302485976</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>0.1781482010377636</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>6</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>11</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>120</v>
+      </c>
+      <c r="BA2" t="inlineStr">
+        <is>
+          <t>B50f</t>
+        </is>
+      </c>
+      <c r="BB2" t="n">
+        <v>300</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>2</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>0.5859375</v>
+      </c>
+      <c r="BE2" t="inlineStr"/>
+      <c r="BF2" t="inlineStr"/>
+      <c r="BG2" t="inlineStr"/>
+      <c r="BH2" t="inlineStr"/>
+      <c r="BI2" t="inlineStr"/>
+      <c r="BJ2" t="inlineStr">
+        <is>
+          <t>19990102</t>
+        </is>
+      </c>
+      <c r="BK2" t="n">
+        <v>500</v>
+      </c>
+      <c r="BL2" t="inlineStr"/>
+      <c r="BM2" t="inlineStr">
+        <is>
+          <t>100012_01-02-1999_3</t>
+        </is>
+      </c>
+      <c r="BN2" t="inlineStr">
+        <is>
+          <t>512x512</t>
+        </is>
+      </c>
+      <c r="BO2" t="inlineStr"/>
+      <c r="BP2" t="inlineStr">
+        <is>
+          <t>NLST-LSS</t>
+        </is>
+      </c>
+      <c r="BQ2" t="inlineStr">
+        <is>
+          <t>D:\Abstract ECR\Data\LDCT - NLST\100012\100012_01-02-1999_3</t>
+        </is>
+      </c>
+      <c r="BR2" t="inlineStr">
+        <is>
+          <t>608762</t>
+        </is>
+      </c>
+      <c r="BS2" t="inlineStr">
         <is>
           <t>SIEMENS</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>SOMATOM Force</t>
-        </is>
-      </c>
-      <c r="N2" t="n">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>GNL 10 SLICE</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>10</v>
-      </c>
-      <c r="D3" t="n">
-        <v>130.9</v>
-      </c>
-      <c r="E3" t="n">
-        <v>122.9613353863726</v>
-      </c>
-      <c r="F3" t="n">
-        <v>44.48638906461505</v>
-      </c>
-      <c r="G3" t="n">
-        <v>4.071368516985725</v>
-      </c>
-      <c r="H3" t="n">
-        <v>100</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Br40d</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>CT11_Soft</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>D:\Ani Nikoghosyan - CT11 vs CT14\Data\Studie_001\CT11_Soft</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>SIEMENS</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>SOMATOM Force</t>
-        </is>
-      </c>
-      <c r="N3" t="n">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>GNL 10 SLICE</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>10</v>
-      </c>
-      <c r="D4" t="n">
-        <v>38.9</v>
-      </c>
-      <c r="E4" t="n">
-        <v>18.65180956368577</v>
-      </c>
-      <c r="F4" t="n">
-        <v>6.003067895637413</v>
-      </c>
-      <c r="G4" t="n">
-        <v>3.722010148867418</v>
-      </c>
-      <c r="H4" t="n">
-        <v>120</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Bl56f</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>CT14_Lung</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>D:\Ani Nikoghosyan - CT11 vs CT14\Data\Studie_001\CT14_Lung</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Siemens Healthineers</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>NAEOTOM Alpha</t>
-        </is>
-      </c>
-      <c r="N4" t="n">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>GNL 10 SLICE</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>10</v>
-      </c>
-      <c r="D5" t="n">
-        <v>39.1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>18.96549498431296</v>
-      </c>
-      <c r="F5" t="n">
-        <v>6.498821079299242</v>
-      </c>
-      <c r="G5" t="n">
-        <v>3.741648288920148</v>
-      </c>
-      <c r="H5" t="n">
-        <v>120</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Br40f</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>CT14_Soft</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>D:\Ani Nikoghosyan - CT11 vs CT14\Data\Studie_001\CT14_Soft</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Siemens Healthineers</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>NAEOTOM Alpha</t>
-        </is>
-      </c>
-      <c r="N5" t="n">
-        <v>144</v>
+      <c r="BT2" t="inlineStr">
+        <is>
+          <t>Volume Zoom</t>
+        </is>
+      </c>
+      <c r="BU2" t="inlineStr">
+        <is>
+          <t>S05</t>
+        </is>
+      </c>
+      <c r="BV2" t="inlineStr"/>
+      <c r="BW2" t="inlineStr">
+        <is>
+          <t>VA40C</t>
+        </is>
+      </c>
+      <c r="BX2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BY2" t="inlineStr"/>
+      <c r="BZ2" t="inlineStr"/>
+      <c r="CA2" t="inlineStr"/>
+      <c r="CB2" t="inlineStr"/>
+      <c r="CC2" t="inlineStr">
+        <is>
+          <t>CHEST</t>
+        </is>
+      </c>
+      <c r="CD2" t="inlineStr">
+        <is>
+          <t>100012</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>